<commit_message>
Changes in Admin and sample.xlsx
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\XAMPP\htdocs\Engineering\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Engineering\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7190" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7188" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="admin" sheetId="8" r:id="rId1"/>
@@ -21,11 +21,11 @@
     <sheet name="lecturer" sheetId="28" r:id="rId7"/>
     <sheet name="subject" sheetId="27" r:id="rId8"/>
     <sheet name="schedule" sheetId="26" r:id="rId9"/>
-    <sheet name="topic" sheetId="18" r:id="rId10"/>
-    <sheet name="announcement" sheetId="33" r:id="rId11"/>
-    <sheet name="activity_details" sheetId="17" r:id="rId12"/>
-    <sheet name="activity" sheetId="7" r:id="rId13"/>
-    <sheet name="lecturer_attendance" sheetId="10" r:id="rId14"/>
+    <sheet name="lecturer_attendance" sheetId="10" r:id="rId10"/>
+    <sheet name="topic" sheetId="18" r:id="rId11"/>
+    <sheet name="announcement" sheetId="33" r:id="rId12"/>
+    <sheet name="activity_details" sheetId="17" r:id="rId13"/>
+    <sheet name="activity" sheetId="7" r:id="rId14"/>
     <sheet name="student" sheetId="5" r:id="rId15"/>
     <sheet name="lecturer_feedback" sheetId="11" r:id="rId16"/>
     <sheet name="log_content" sheetId="32" r:id="rId17"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="254">
   <si>
     <t>lecturer_id</t>
   </si>
@@ -807,7 +807,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1136,25 +1136,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.90625" customWidth="1"/>
-    <col min="2" max="2" width="12.26953125" customWidth="1"/>
-    <col min="3" max="3" width="12.08984375" customWidth="1"/>
-    <col min="4" max="4" width="13.1796875" customWidth="1"/>
-    <col min="5" max="5" width="11.6328125" customWidth="1"/>
-    <col min="6" max="6" width="11.1796875" customWidth="1"/>
-    <col min="7" max="7" width="12.08984375" customWidth="1"/>
+    <col min="1" max="1" width="9.88671875" customWidth="1"/>
+    <col min="2" max="2" width="12.21875" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" customWidth="1"/>
+    <col min="4" max="4" width="13.21875" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" customWidth="1"/>
+    <col min="6" max="6" width="11.21875" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>58</v>
       </c>
@@ -1177,7 +1177,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>202011111</v>
       </c>
@@ -1207,23 +1207,138 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.88671875" customWidth="1"/>
+    <col min="2" max="2" width="24.5546875" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" customWidth="1"/>
+    <col min="6" max="6" width="11.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1515455338</v>
+      </c>
+      <c r="C2">
+        <v>1515455338</v>
+      </c>
+      <c r="D2">
+        <v>1515476979</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1515479755</v>
+      </c>
+      <c r="C3">
+        <v>1515479755</v>
+      </c>
+      <c r="D3">
+        <v>1515503216</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1518166800</v>
+      </c>
+      <c r="C4">
+        <v>1518166800</v>
+      </c>
+      <c r="D4">
+        <v>1518174000</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.54296875" customWidth="1"/>
-    <col min="2" max="2" width="15.453125" customWidth="1"/>
-    <col min="3" max="3" width="19.81640625" customWidth="1"/>
-    <col min="4" max="4" width="13.453125" customWidth="1"/>
-    <col min="5" max="5" width="11.36328125" customWidth="1"/>
+    <col min="1" max="1" width="9.5546875" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" customWidth="1"/>
+    <col min="3" max="3" width="19.77734375" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>53</v>
       </c>
@@ -1240,7 +1355,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1257,7 +1372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1274,7 +1389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1291,7 +1406,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1313,26 +1428,26 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.453125" customWidth="1"/>
-    <col min="3" max="3" width="14.54296875" customWidth="1"/>
-    <col min="4" max="4" width="12.26953125" customWidth="1"/>
-    <col min="5" max="5" width="15.08984375" customWidth="1"/>
-    <col min="6" max="6" width="22.90625" customWidth="1"/>
-    <col min="7" max="7" width="23.453125" customWidth="1"/>
-    <col min="8" max="8" width="23.7265625" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" customWidth="1"/>
+    <col min="4" max="4" width="12.21875" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" customWidth="1"/>
+    <col min="6" max="6" width="22.88671875" customWidth="1"/>
+    <col min="7" max="7" width="23.44140625" customWidth="1"/>
+    <col min="8" max="8" width="23.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>63</v>
       </c>
@@ -1358,7 +1473,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1389,21 +1504,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.6328125" customWidth="1"/>
-    <col min="2" max="2" width="20.7265625" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -1411,7 +1526,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1419,7 +1534,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1427,7 +1542,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1440,25 +1555,25 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.54296875" customWidth="1"/>
-    <col min="2" max="2" width="18.26953125" customWidth="1"/>
-    <col min="3" max="3" width="16.90625" customWidth="1"/>
-    <col min="4" max="4" width="14.81640625" customWidth="1"/>
-    <col min="5" max="5" width="19.7265625" customWidth="1"/>
-    <col min="6" max="6" width="15.7265625" customWidth="1"/>
+    <col min="1" max="1" width="12.5546875" customWidth="1"/>
+    <col min="2" max="2" width="18.21875" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" customWidth="1"/>
+    <col min="4" max="4" width="14.77734375" customWidth="1"/>
+    <col min="5" max="5" width="19.77734375" customWidth="1"/>
+    <col min="6" max="6" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>48</v>
       </c>
@@ -1481,7 +1596,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1504,7 +1619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1524,89 +1639,6 @@
         <v>2</v>
       </c>
       <c r="G3">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="20.90625" customWidth="1"/>
-    <col min="2" max="2" width="24.54296875" customWidth="1"/>
-    <col min="3" max="3" width="20.453125" customWidth="1"/>
-    <col min="4" max="4" width="22.6328125" customWidth="1"/>
-    <col min="5" max="5" width="11.90625" customWidth="1"/>
-    <col min="6" max="6" width="11.453125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1515455338</v>
-      </c>
-      <c r="C2">
-        <v>1515455338</v>
-      </c>
-      <c r="D2">
-        <v>1515476979</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>1515479755</v>
-      </c>
-      <c r="C3">
-        <v>1515479755</v>
-      </c>
-      <c r="D3">
-        <v>1515503216</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
         <v>2</v>
       </c>
     </row>
@@ -1616,28 +1648,28 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.54296875" customWidth="1"/>
-    <col min="2" max="2" width="16.54296875" customWidth="1"/>
-    <col min="3" max="3" width="16.6328125" customWidth="1"/>
-    <col min="4" max="4" width="16.453125" customWidth="1"/>
-    <col min="5" max="5" width="12.1796875" customWidth="1"/>
-    <col min="6" max="6" width="15.08984375" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.44140625" customWidth="1"/>
+    <col min="5" max="5" width="12.21875" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" customWidth="1"/>
     <col min="7" max="7" width="22" customWidth="1"/>
-    <col min="8" max="8" width="18.54296875" customWidth="1"/>
-    <col min="9" max="9" width="46.453125" customWidth="1"/>
-    <col min="10" max="10" width="12.453125" customWidth="1"/>
+    <col min="8" max="8" width="18.5546875" customWidth="1"/>
+    <col min="9" max="9" width="46.44140625" customWidth="1"/>
+    <col min="10" max="10" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -1669,7 +1701,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>201511281</v>
       </c>
@@ -1701,7 +1733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>201511438</v>
       </c>
@@ -1733,7 +1765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>201411491</v>
       </c>
@@ -1765,7 +1797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>201410679</v>
       </c>
@@ -1797,7 +1829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>201411851</v>
       </c>
@@ -1829,7 +1861,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>201410215</v>
       </c>
@@ -1861,7 +1893,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>201420096</v>
       </c>
@@ -1893,7 +1925,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>201512590</v>
       </c>
@@ -1925,7 +1957,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>201411823</v>
       </c>
@@ -1957,7 +1989,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>201410617</v>
       </c>
@@ -1989,7 +2021,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>201410881</v>
       </c>
@@ -2021,7 +2053,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>201512068</v>
       </c>
@@ -2053,7 +2085,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>201512491</v>
       </c>
@@ -2085,7 +2117,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>201510652</v>
       </c>
@@ -2117,7 +2149,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>201511230</v>
       </c>
@@ -2149,7 +2181,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>201511911</v>
       </c>
@@ -2181,7 +2213,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>201510573</v>
       </c>
@@ -2213,7 +2245,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>201512532</v>
       </c>
@@ -2245,7 +2277,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>201510186</v>
       </c>
@@ -2279,10 +2311,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
-    <hyperlink ref="G3" r:id="rId2"/>
-    <hyperlink ref="G4:G7" r:id="rId3" display="adre@fit.edu.ph"/>
-    <hyperlink ref="G8:G20" r:id="rId4" display="adre@fit.edu.ph"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0E00-000000000000}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-0E00-000001000000}"/>
+    <hyperlink ref="G4:G7" r:id="rId3" display="adre@fit.edu.ph" xr:uid="{00000000-0004-0000-0E00-000002000000}"/>
+    <hyperlink ref="G8:G20" r:id="rId4" display="adre@fit.edu.ph" xr:uid="{00000000-0004-0000-0E00-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId5"/>
@@ -2290,26 +2322,26 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.7265625" customWidth="1"/>
-    <col min="2" max="2" width="25.08984375" customWidth="1"/>
-    <col min="3" max="3" width="25.6328125" customWidth="1"/>
+    <col min="1" max="1" width="20.77734375" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" customWidth="1"/>
     <col min="4" max="4" width="28" customWidth="1"/>
-    <col min="5" max="5" width="11.08984375" customWidth="1"/>
-    <col min="6" max="6" width="11.1796875" customWidth="1"/>
-    <col min="7" max="7" width="14.08984375" customWidth="1"/>
-    <col min="8" max="8" width="10.7265625" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" customWidth="1"/>
+    <col min="6" max="6" width="11.21875" customWidth="1"/>
+    <col min="7" max="7" width="14.109375" customWidth="1"/>
+    <col min="8" max="8" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>77</v>
       </c>
@@ -2335,7 +2367,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2361,7 +2393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2387,7 +2419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2413,7 +2445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2439,7 +2471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2465,7 +2497,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2497,20 +2529,20 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.6328125" customWidth="1"/>
-    <col min="2" max="2" width="17.90625" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>242</v>
       </c>
@@ -2518,7 +2550,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2532,22 +2564,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.26953125" customWidth="1"/>
-    <col min="2" max="2" width="13.26953125" customWidth="1"/>
-    <col min="3" max="3" width="15.26953125" customWidth="1"/>
-    <col min="4" max="4" width="19.6328125" customWidth="1"/>
+    <col min="1" max="1" width="12.21875" customWidth="1"/>
+    <col min="2" max="2" width="13.21875" customWidth="1"/>
+    <col min="3" max="3" width="15.21875" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -2561,7 +2593,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2575,7 +2607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2596,28 +2628,28 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="I2" sqref="I2:I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="18.90625" customWidth="1"/>
-    <col min="4" max="4" width="20.453125" customWidth="1"/>
-    <col min="5" max="5" width="22.7265625" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" customWidth="1"/>
+    <col min="4" max="4" width="20.44140625" customWidth="1"/>
+    <col min="5" max="5" width="22.77734375" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
-    <col min="7" max="7" width="12.26953125" customWidth="1"/>
-    <col min="8" max="8" width="9.90625" customWidth="1"/>
+    <col min="7" max="7" width="12.21875" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" customWidth="1"/>
     <col min="9" max="9" width="29" customWidth="1"/>
-    <col min="10" max="10" width="23.6328125" customWidth="1"/>
+    <col min="10" max="10" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -2649,7 +2681,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>201111111</v>
       </c>
@@ -2681,7 +2713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>201122222</v>
       </c>
@@ -2713,7 +2745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>201133333</v>
       </c>
@@ -2745,7 +2777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>201144444</v>
       </c>
@@ -2779,10 +2811,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="F3" r:id="rId2"/>
-    <hyperlink ref="F4" r:id="rId3"/>
-    <hyperlink ref="F5" r:id="rId4"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId5"/>
@@ -2790,24 +2822,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.26953125" customWidth="1"/>
-    <col min="2" max="2" width="21.453125" customWidth="1"/>
-    <col min="3" max="3" width="25.90625" customWidth="1"/>
-    <col min="4" max="4" width="21.90625" customWidth="1"/>
-    <col min="5" max="5" width="14.26953125" customWidth="1"/>
-    <col min="6" max="6" width="16.81640625" customWidth="1"/>
+    <col min="1" max="1" width="12.21875" customWidth="1"/>
+    <col min="2" max="2" width="21.44140625" customWidth="1"/>
+    <col min="3" max="3" width="25.88671875" customWidth="1"/>
+    <col min="4" max="4" width="21.88671875" customWidth="1"/>
+    <col min="5" max="5" width="14.21875" customWidth="1"/>
+    <col min="6" max="6" width="16.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>192</v>
       </c>
@@ -2827,7 +2859,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2847,7 +2879,7 @@
         <v>201111111</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2867,7 +2899,7 @@
         <v>201122222</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2887,7 +2919,7 @@
         <v>201133333</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2914,25 +2946,25 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="10.1796875" customWidth="1"/>
-    <col min="4" max="4" width="10.54296875" customWidth="1"/>
-    <col min="5" max="5" width="10.36328125" customWidth="1"/>
-    <col min="6" max="6" width="11.36328125" customWidth="1"/>
-    <col min="7" max="7" width="22.08984375" customWidth="1"/>
-    <col min="8" max="8" width="21.08984375" customWidth="1"/>
-    <col min="9" max="9" width="14.1796875" customWidth="1"/>
+    <col min="3" max="3" width="10.21875" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" customWidth="1"/>
+    <col min="7" max="7" width="22.109375" customWidth="1"/>
+    <col min="8" max="8" width="21.109375" customWidth="1"/>
+    <col min="9" max="9" width="14.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>203</v>
       </c>
@@ -2964,7 +2996,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2996,7 +3028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3028,7 +3060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3060,7 +3092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3094,31 +3126,31 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
-    <hyperlink ref="G3" r:id="rId2"/>
-    <hyperlink ref="G4" r:id="rId3"/>
-    <hyperlink ref="G5" r:id="rId4"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
+    <hyperlink ref="G5" r:id="rId4" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.54296875" customWidth="1"/>
-    <col min="2" max="2" width="14.6328125" customWidth="1"/>
-    <col min="3" max="3" width="18.6328125" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>39</v>
       </c>
@@ -3135,7 +3167,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3152,7 +3184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3169,7 +3201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3186,7 +3218,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3203,7 +3235,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3220,7 +3252,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3237,7 +3269,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3254,7 +3286,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3277,28 +3309,28 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.36328125" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="10.453125" customWidth="1"/>
-    <col min="4" max="4" width="11.7265625" customWidth="1"/>
-    <col min="5" max="5" width="10.6328125" customWidth="1"/>
-    <col min="6" max="6" width="17.26953125" customWidth="1"/>
-    <col min="7" max="7" width="21.6328125" customWidth="1"/>
-    <col min="8" max="8" width="14.36328125" customWidth="1"/>
-    <col min="9" max="9" width="13.36328125" customWidth="1"/>
-    <col min="10" max="10" width="11.54296875" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" customWidth="1"/>
+    <col min="4" max="4" width="11.77734375" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" customWidth="1"/>
+    <col min="6" max="6" width="17.21875" customWidth="1"/>
+    <col min="7" max="7" width="21.6640625" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" customWidth="1"/>
+    <col min="10" max="10" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3330,7 +3362,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3362,7 +3394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3394,7 +3426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3426,7 +3458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3460,10 +3492,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
-    <hyperlink ref="G3" r:id="rId2"/>
-    <hyperlink ref="G4" r:id="rId3"/>
-    <hyperlink ref="G5" r:id="rId4"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
+    <hyperlink ref="G5" r:id="rId4" xr:uid="{00000000-0004-0000-0600-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId5"/>
@@ -3471,23 +3503,23 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.36328125" customWidth="1"/>
-    <col min="2" max="2" width="16.81640625" customWidth="1"/>
-    <col min="3" max="3" width="18.1796875" customWidth="1"/>
-    <col min="4" max="4" width="15.7265625" customWidth="1"/>
-    <col min="5" max="5" width="10.6328125" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.77734375" customWidth="1"/>
+    <col min="3" max="3" width="18.21875" customWidth="1"/>
+    <col min="4" max="4" width="15.77734375" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>98</v>
       </c>
@@ -3504,7 +3536,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3521,7 +3553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3538,7 +3570,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3555,7 +3587,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3572,7 +3604,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3589,7 +3621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3606,7 +3638,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3623,7 +3655,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3646,24 +3678,24 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.453125" customWidth="1"/>
-    <col min="2" max="2" width="20.90625" customWidth="1"/>
-    <col min="3" max="3" width="21.08984375" customWidth="1"/>
-    <col min="4" max="4" width="17.1796875" customWidth="1"/>
-    <col min="5" max="5" width="14.7265625" customWidth="1"/>
-    <col min="6" max="6" width="19.90625" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" customWidth="1"/>
+    <col min="3" max="3" width="21.109375" customWidth="1"/>
+    <col min="4" max="4" width="17.21875" customWidth="1"/>
+    <col min="5" max="5" width="14.77734375" customWidth="1"/>
+    <col min="6" max="6" width="19.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>81</v>
       </c>
@@ -3683,15 +3715,15 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>28800</v>
+        <v>1517958000</v>
       </c>
       <c r="C2">
-        <v>39600</v>
+        <v>1517968200</v>
       </c>
       <c r="D2" t="s">
         <v>85</v>
@@ -3703,15 +3735,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>43200</v>
+        <v>1518066000</v>
       </c>
       <c r="C3">
-        <v>54000</v>
+        <v>1518073200</v>
       </c>
       <c r="D3" t="s">
         <v>86</v>
@@ -3723,15 +3755,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>28800</v>
+        <v>1518166800</v>
       </c>
       <c r="C4">
-        <v>39600</v>
+        <v>1518174000</v>
       </c>
       <c r="D4" t="s">
         <v>85</v>
@@ -3743,15 +3775,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>43200</v>
+        <v>1518231600</v>
       </c>
       <c r="C5">
-        <v>54000</v>
+        <v>1518238800</v>
       </c>
       <c r="D5" t="s">
         <v>86</v>

</xml_diff>